<commit_message>
feat: implement main/sub auto set and generation
</commit_message>
<xml_diff>
--- a/Categories.xlsx
+++ b/Categories.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,25 +421,37 @@
       <c r="F1" t="str">
         <v>slug.en-US</v>
       </c>
+      <c r="G1" t="str">
+        <v>parent.key</v>
+      </c>
+      <c r="H1" t="str">
+        <v>parent.typeId</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>category</v>
       </c>
       <c r="B2" t="str">
-        <v>Advanced-ExpertKey</v>
+        <v>abilityLevelKey</v>
       </c>
       <c r="C2" t="str">
-        <v>Advanced-ExpertDescription</v>
+        <v>abilityLevelDescription</v>
       </c>
       <c r="D2" t="str">
-        <v>Advanced-ExpertId</v>
+        <v>abilityLevelId</v>
       </c>
       <c r="E2" t="str">
-        <v>Advanced-Expert</v>
+        <v>AbilityLevel</v>
       </c>
       <c r="F2" t="str">
-        <v>Advanced-ExpertSlug</v>
+        <v>abilityLevelSlug</v>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -447,19 +459,25 @@
         <v>category</v>
       </c>
       <c r="B3" t="str">
-        <v>LibTechKey</v>
+        <v>brandKey</v>
       </c>
       <c r="C3" t="str">
-        <v>LibTechDescription</v>
+        <v>brandDescription</v>
       </c>
       <c r="D3" t="str">
-        <v>LibTechId</v>
+        <v>brandId</v>
       </c>
       <c r="E3" t="str">
-        <v>LibTech</v>
+        <v>Brand</v>
       </c>
       <c r="F3" t="str">
-        <v>LibTechSlug</v>
+        <v>brandSlug</v>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -467,19 +485,25 @@
         <v>category</v>
       </c>
       <c r="B4" t="str">
-        <v>adult-maleKey</v>
+        <v>ageGroupKey</v>
       </c>
       <c r="C4" t="str">
-        <v>adult-maleDescription</v>
+        <v>ageGroupDescription</v>
       </c>
       <c r="D4" t="str">
-        <v>adult-maleId</v>
+        <v>ageGroupId</v>
       </c>
       <c r="E4" t="str">
-        <v>Adult-male</v>
+        <v>AgeGroup</v>
       </c>
       <c r="F4" t="str">
-        <v>adult-maleSlug</v>
+        <v>ageGroupSlug</v>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -487,19 +511,25 @@
         <v>category</v>
       </c>
       <c r="B5" t="str">
-        <v>FreestyleKey</v>
+        <v>terrainKey</v>
       </c>
       <c r="C5" t="str">
-        <v>FreestyleDescription</v>
+        <v>terrainDescription</v>
       </c>
       <c r="D5" t="str">
-        <v>FreestyleId</v>
+        <v>terrainId</v>
       </c>
       <c r="E5" t="str">
-        <v>Freestyle</v>
+        <v>Terrain</v>
       </c>
       <c r="F5" t="str">
-        <v>FreestyleSlug</v>
+        <v>terrainSlug</v>
+      </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <v/>
       </c>
     </row>
     <row r="6">
@@ -507,19 +537,25 @@
         <v>category</v>
       </c>
       <c r="B6" t="str">
-        <v>All-MountainKey</v>
+        <v>Advanced-ExpertKey</v>
       </c>
       <c r="C6" t="str">
-        <v>All-MountainDescription</v>
+        <v>Advanced-ExpertDescription</v>
       </c>
       <c r="D6" t="str">
-        <v>All-MountainId</v>
+        <v>Advanced-ExpertId</v>
       </c>
       <c r="E6" t="str">
-        <v>All-Mountain</v>
+        <v>Advanced-Expert</v>
       </c>
       <c r="F6" t="str">
-        <v>All-MountainSlug</v>
+        <v>Advanced-ExpertSlug</v>
+      </c>
+      <c r="G6" t="str">
+        <v>abilityLevelKey</v>
+      </c>
+      <c r="H6" t="str">
+        <v>category</v>
       </c>
     </row>
     <row r="7">
@@ -527,19 +563,25 @@
         <v>category</v>
       </c>
       <c r="B7" t="str">
-        <v>FreerideKey</v>
+        <v>LibTechKey</v>
       </c>
       <c r="C7" t="str">
-        <v>FreerideDescription</v>
+        <v>LibTechDescription</v>
       </c>
       <c r="D7" t="str">
-        <v>FreerideId</v>
+        <v>LibTechId</v>
       </c>
       <c r="E7" t="str">
-        <v>Freeride</v>
+        <v>LibTech</v>
       </c>
       <c r="F7" t="str">
-        <v>FreerideSlug</v>
+        <v>LibTechSlug</v>
+      </c>
+      <c r="G7" t="str">
+        <v>brandKey</v>
+      </c>
+      <c r="H7" t="str">
+        <v>category</v>
       </c>
     </row>
     <row r="8">
@@ -547,19 +589,25 @@
         <v>category</v>
       </c>
       <c r="B8" t="str">
-        <v>Intermediate-AdvancedKey</v>
+        <v>adult-maleKey</v>
       </c>
       <c r="C8" t="str">
-        <v>Intermediate-AdvancedDescription</v>
+        <v>adult-maleDescription</v>
       </c>
       <c r="D8" t="str">
-        <v>Intermediate-AdvancedId</v>
+        <v>adult-maleId</v>
       </c>
       <c r="E8" t="str">
-        <v>Intermediate-Advanced</v>
+        <v>Adult-male</v>
       </c>
       <c r="F8" t="str">
-        <v>Intermediate-AdvancedSlug</v>
+        <v>adult-maleSlug</v>
+      </c>
+      <c r="G8" t="str">
+        <v>ageGroupKey</v>
+      </c>
+      <c r="H8" t="str">
+        <v>category</v>
       </c>
     </row>
     <row r="9">
@@ -567,19 +615,25 @@
         <v>category</v>
       </c>
       <c r="B9" t="str">
-        <v>RideKey</v>
+        <v>FreestyleKey</v>
       </c>
       <c r="C9" t="str">
-        <v>RideDescription</v>
+        <v>FreestyleDescription</v>
       </c>
       <c r="D9" t="str">
-        <v>RideId</v>
+        <v>FreestyleId</v>
       </c>
       <c r="E9" t="str">
-        <v>Ride</v>
+        <v>Freestyle</v>
       </c>
       <c r="F9" t="str">
-        <v>RideSlug</v>
+        <v>FreestyleSlug</v>
+      </c>
+      <c r="G9" t="str">
+        <v>terrainKey</v>
+      </c>
+      <c r="H9" t="str">
+        <v>category</v>
       </c>
     </row>
     <row r="10">
@@ -587,24 +641,316 @@
         <v>category</v>
       </c>
       <c r="B10" t="str">
+        <v>All-MountainKey</v>
+      </c>
+      <c r="C10" t="str">
+        <v>All-MountainDescription</v>
+      </c>
+      <c r="D10" t="str">
+        <v>All-MountainId</v>
+      </c>
+      <c r="E10" t="str">
+        <v>All-Mountain</v>
+      </c>
+      <c r="F10" t="str">
+        <v>All-MountainSlug</v>
+      </c>
+      <c r="G10" t="str">
+        <v>terrainKey</v>
+      </c>
+      <c r="H10" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>category</v>
+      </c>
+      <c r="B11" t="str">
+        <v>FreerideKey</v>
+      </c>
+      <c r="C11" t="str">
+        <v>FreerideDescription</v>
+      </c>
+      <c r="D11" t="str">
+        <v>FreerideId</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Freeride</v>
+      </c>
+      <c r="F11" t="str">
+        <v>FreerideSlug</v>
+      </c>
+      <c r="G11" t="str">
+        <v>terrainKey</v>
+      </c>
+      <c r="H11" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>category</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Intermediate-AdvancedKey</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Intermediate-AdvancedDescription</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Intermediate-AdvancedId</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Intermediate-Advanced</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Intermediate-AdvancedSlug</v>
+      </c>
+      <c r="G12" t="str">
+        <v>abilityLevelKey</v>
+      </c>
+      <c r="H12" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>category</v>
+      </c>
+      <c r="B13" t="str">
+        <v>RideKey</v>
+      </c>
+      <c r="C13" t="str">
+        <v>RideDescription</v>
+      </c>
+      <c r="D13" t="str">
+        <v>RideId</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Ride</v>
+      </c>
+      <c r="F13" t="str">
+        <v>RideSlug</v>
+      </c>
+      <c r="G13" t="str">
+        <v>brandKey</v>
+      </c>
+      <c r="H13" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>category</v>
+      </c>
+      <c r="B14" t="str">
         <v>adult-anyKey</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C14" t="str">
         <v>adult-anyDescription</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D14" t="str">
         <v>adult-anyId</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E14" t="str">
         <v>Adult-any</v>
       </c>
-      <c r="F10" t="str">
+      <c r="F14" t="str">
         <v>adult-anySlug</v>
+      </c>
+      <c r="G14" t="str">
+        <v>ageGroupKey</v>
+      </c>
+      <c r="H14" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>category</v>
+      </c>
+      <c r="B15" t="str">
+        <v>CAPiTAKey</v>
+      </c>
+      <c r="C15" t="str">
+        <v>CAPiTADescription</v>
+      </c>
+      <c r="D15" t="str">
+        <v>CAPiTAId</v>
+      </c>
+      <c r="E15" t="str">
+        <v>CAPiTA</v>
+      </c>
+      <c r="F15" t="str">
+        <v>CAPiTASlug</v>
+      </c>
+      <c r="G15" t="str">
+        <v>brandKey</v>
+      </c>
+      <c r="H15" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>category</v>
+      </c>
+      <c r="B16" t="str">
+        <v>SeasonKey</v>
+      </c>
+      <c r="C16" t="str">
+        <v>SeasonDescription</v>
+      </c>
+      <c r="D16" t="str">
+        <v>SeasonId</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Season</v>
+      </c>
+      <c r="F16" t="str">
+        <v>SeasonSlug</v>
+      </c>
+      <c r="G16" t="str">
+        <v>brandKey</v>
+      </c>
+      <c r="H16" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>category</v>
+      </c>
+      <c r="B17" t="str">
+        <v>PowderKey</v>
+      </c>
+      <c r="C17" t="str">
+        <v>PowderDescription</v>
+      </c>
+      <c r="D17" t="str">
+        <v>PowderId</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Powder</v>
+      </c>
+      <c r="F17" t="str">
+        <v>PowderSlug</v>
+      </c>
+      <c r="G17" t="str">
+        <v>terrainKey</v>
+      </c>
+      <c r="H17" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>category</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Beginner-IntermediateKey</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Beginner-IntermediateDescription</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Beginner-IntermediateId</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Beginner-Intermediate</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Beginner-IntermediateSlug</v>
+      </c>
+      <c r="G18" t="str">
+        <v>abilityLevelKey</v>
+      </c>
+      <c r="H18" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>category</v>
+      </c>
+      <c r="B19" t="str">
+        <v>RossignolKey</v>
+      </c>
+      <c r="C19" t="str">
+        <v>RossignolDescription</v>
+      </c>
+      <c r="D19" t="str">
+        <v>RossignolId</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Rossignol</v>
+      </c>
+      <c r="F19" t="str">
+        <v>RossignolSlug</v>
+      </c>
+      <c r="G19" t="str">
+        <v>brandKey</v>
+      </c>
+      <c r="H19" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>category</v>
+      </c>
+      <c r="B20" t="str">
+        <v>adult-femaleKey</v>
+      </c>
+      <c r="C20" t="str">
+        <v>adult-femaleDescription</v>
+      </c>
+      <c r="D20" t="str">
+        <v>adult-femaleId</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Adult-female</v>
+      </c>
+      <c r="F20" t="str">
+        <v>adult-femaleSlug</v>
+      </c>
+      <c r="G20" t="str">
+        <v>ageGroupKey</v>
+      </c>
+      <c r="H20" t="str">
+        <v>category</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>category</v>
+      </c>
+      <c r="B21" t="str">
+        <v>K2Key</v>
+      </c>
+      <c r="C21" t="str">
+        <v>K2Description</v>
+      </c>
+      <c r="D21" t="str">
+        <v>K2Id</v>
+      </c>
+      <c r="E21" t="str">
+        <v>K2</v>
+      </c>
+      <c r="F21" t="str">
+        <v>K2Slug</v>
+      </c>
+      <c r="G21" t="str">
+        <v>brandKey</v>
+      </c>
+      <c r="H21" t="str">
+        <v>category</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: fix bad formatting
</commit_message>
<xml_diff>
--- a/Categories.xlsx
+++ b/Categories.xlsx
@@ -1083,22 +1083,22 @@
         <v>category</v>
       </c>
       <c r="B27" t="str">
-        <v>YesKey</v>
+        <v>child-anyKey</v>
       </c>
       <c r="C27" t="str">
-        <v>YesDescription</v>
+        <v>child-anyDescription</v>
       </c>
       <c r="D27" t="str">
-        <v>YesId</v>
+        <v>child-anyId</v>
       </c>
       <c r="E27" t="str">
-        <v>Yes</v>
+        <v>Child-any</v>
       </c>
       <c r="F27" t="str">
-        <v>YesSlug</v>
+        <v>child-anySlug</v>
       </c>
       <c r="G27" t="str">
-        <v>brandKey</v>
+        <v>ageGroupKey</v>
       </c>
       <c r="H27" t="str">
         <v>category</v>
@@ -1109,19 +1109,19 @@
         <v>category</v>
       </c>
       <c r="B28" t="str">
-        <v>CardiffKey</v>
+        <v>JonesKey</v>
       </c>
       <c r="C28" t="str">
-        <v>CardiffDescription</v>
+        <v>JonesDescription</v>
       </c>
       <c r="D28" t="str">
-        <v>CardiffId</v>
+        <v>JonesId</v>
       </c>
       <c r="E28" t="str">
-        <v>Cardiff</v>
+        <v>Jones</v>
       </c>
       <c r="F28" t="str">
-        <v>CardiffSlug</v>
+        <v>JonesSlug</v>
       </c>
       <c r="G28" t="str">
         <v>brandKey</v>
@@ -1135,22 +1135,22 @@
         <v>category</v>
       </c>
       <c r="B29" t="str">
-        <v>SplitboardingKey</v>
+        <v>BataleonKey</v>
       </c>
       <c r="C29" t="str">
-        <v>SplitboardingDescription</v>
+        <v>BataleonDescription</v>
       </c>
       <c r="D29" t="str">
-        <v>SplitboardingId</v>
+        <v>BataleonId</v>
       </c>
       <c r="E29" t="str">
-        <v>Splitboarding</v>
+        <v>Bataleon</v>
       </c>
       <c r="F29" t="str">
-        <v>SplitboardingSlug</v>
+        <v>BataleonSlug</v>
       </c>
       <c r="G29" t="str">
-        <v>terrainKey</v>
+        <v>brandKey</v>
       </c>
       <c r="H29" t="str">
         <v>category</v>
@@ -1161,22 +1161,22 @@
         <v>category</v>
       </c>
       <c r="B30" t="str">
-        <v>JonesKey</v>
+        <v>child-boyKey</v>
       </c>
       <c r="C30" t="str">
-        <v>JonesDescription</v>
+        <v>child-boyDescription</v>
       </c>
       <c r="D30" t="str">
-        <v>JonesId</v>
+        <v>child-boyId</v>
       </c>
       <c r="E30" t="str">
-        <v>Jones</v>
+        <v>Child-boy</v>
       </c>
       <c r="F30" t="str">
-        <v>JonesSlug</v>
+        <v>child-boySlug</v>
       </c>
       <c r="G30" t="str">
-        <v>brandKey</v>
+        <v>ageGroupKey</v>
       </c>
       <c r="H30" t="str">
         <v>category</v>
@@ -1187,19 +1187,19 @@
         <v>category</v>
       </c>
       <c r="B31" t="str">
-        <v>WestonKey</v>
+        <v>SalomonKey</v>
       </c>
       <c r="C31" t="str">
-        <v>WestonDescription</v>
+        <v>SalomonDescription</v>
       </c>
       <c r="D31" t="str">
-        <v>WestonId</v>
+        <v>SalomonId</v>
       </c>
       <c r="E31" t="str">
-        <v>Weston</v>
+        <v>Salomon</v>
       </c>
       <c r="F31" t="str">
-        <v>WestonSlug</v>
+        <v>SalomonSlug</v>
       </c>
       <c r="G31" t="str">
         <v>brandKey</v>
@@ -1213,22 +1213,22 @@
         <v>category</v>
       </c>
       <c r="B32" t="str">
-        <v>child-anyKey</v>
+        <v>RomeKey</v>
       </c>
       <c r="C32" t="str">
-        <v>child-anyDescription</v>
+        <v>RomeDescription</v>
       </c>
       <c r="D32" t="str">
-        <v>child-anyId</v>
+        <v>RomeId</v>
       </c>
       <c r="E32" t="str">
-        <v>Child-any</v>
+        <v>Rome</v>
       </c>
       <c r="F32" t="str">
-        <v>child-anySlug</v>
+        <v>RomeSlug</v>
       </c>
       <c r="G32" t="str">
-        <v>ageGroupKey</v>
+        <v>brandKey</v>
       </c>
       <c r="H32" t="str">
         <v>category</v>
@@ -1239,19 +1239,19 @@
         <v>category</v>
       </c>
       <c r="B33" t="str">
-        <v>BataleonKey</v>
+        <v>SimsKey</v>
       </c>
       <c r="C33" t="str">
-        <v>BataleonDescription</v>
+        <v>SimsDescription</v>
       </c>
       <c r="D33" t="str">
-        <v>BataleonId</v>
+        <v>SimsId</v>
       </c>
       <c r="E33" t="str">
-        <v>Bataleon</v>
+        <v>Sims</v>
       </c>
       <c r="F33" t="str">
-        <v>BataleonSlug</v>
+        <v>SimsSlug</v>
       </c>
       <c r="G33" t="str">
         <v>brandKey</v>
@@ -1265,22 +1265,22 @@
         <v>category</v>
       </c>
       <c r="B34" t="str">
-        <v>child-boyKey</v>
+        <v>SplitboardingKey</v>
       </c>
       <c r="C34" t="str">
-        <v>child-boyDescription</v>
+        <v>SplitboardingDescription</v>
       </c>
       <c r="D34" t="str">
-        <v>child-boyId</v>
+        <v>SplitboardingId</v>
       </c>
       <c r="E34" t="str">
-        <v>Child-boy</v>
+        <v>Splitboarding</v>
       </c>
       <c r="F34" t="str">
-        <v>child-boySlug</v>
+        <v>SplitboardingSlug</v>
       </c>
       <c r="G34" t="str">
-        <v>ageGroupKey</v>
+        <v>terrainKey</v>
       </c>
       <c r="H34" t="str">
         <v>category</v>
@@ -1291,19 +1291,19 @@
         <v>category</v>
       </c>
       <c r="B35" t="str">
-        <v>SalomonKey</v>
+        <v>NitroKey</v>
       </c>
       <c r="C35" t="str">
-        <v>SalomonDescription</v>
+        <v>NitroDescription</v>
       </c>
       <c r="D35" t="str">
-        <v>SalomonId</v>
+        <v>NitroId</v>
       </c>
       <c r="E35" t="str">
-        <v>Salomon</v>
+        <v>Nitro</v>
       </c>
       <c r="F35" t="str">
-        <v>SalomonSlug</v>
+        <v>NitroSlug</v>
       </c>
       <c r="G35" t="str">
         <v>brandKey</v>
@@ -1317,19 +1317,19 @@
         <v>category</v>
       </c>
       <c r="B36" t="str">
-        <v>RomeKey</v>
+        <v>NeverSummerKey</v>
       </c>
       <c r="C36" t="str">
-        <v>RomeDescription</v>
+        <v>NeverSummerDescription</v>
       </c>
       <c r="D36" t="str">
-        <v>RomeId</v>
+        <v>NeverSummerId</v>
       </c>
       <c r="E36" t="str">
-        <v>Rome</v>
+        <v>NeverSummer</v>
       </c>
       <c r="F36" t="str">
-        <v>RomeSlug</v>
+        <v>NeverSummerSlug</v>
       </c>
       <c r="G36" t="str">
         <v>brandKey</v>
@@ -1343,22 +1343,22 @@
         <v>category</v>
       </c>
       <c r="B37" t="str">
-        <v>SimsKey</v>
+        <v>child-girlKey</v>
       </c>
       <c r="C37" t="str">
-        <v>SimsDescription</v>
+        <v>child-girlDescription</v>
       </c>
       <c r="D37" t="str">
-        <v>SimsId</v>
+        <v>child-girlId</v>
       </c>
       <c r="E37" t="str">
-        <v>Sims</v>
+        <v>Child-girl</v>
       </c>
       <c r="F37" t="str">
-        <v>SimsSlug</v>
+        <v>child-girlSlug</v>
       </c>
       <c r="G37" t="str">
-        <v>brandKey</v>
+        <v>ageGroupKey</v>
       </c>
       <c r="H37" t="str">
         <v>category</v>
@@ -1369,19 +1369,19 @@
         <v>category</v>
       </c>
       <c r="B38" t="str">
-        <v>NitroKey</v>
+        <v>UnitedShapesKey</v>
       </c>
       <c r="C38" t="str">
-        <v>NitroDescription</v>
+        <v>UnitedShapesDescription</v>
       </c>
       <c r="D38" t="str">
-        <v>NitroId</v>
+        <v>UnitedShapesId</v>
       </c>
       <c r="E38" t="str">
-        <v>Nitro</v>
+        <v>UnitedShapes</v>
       </c>
       <c r="F38" t="str">
-        <v>NitroSlug</v>
+        <v>UnitedShapesSlug</v>
       </c>
       <c r="G38" t="str">
         <v>brandKey</v>
@@ -1395,22 +1395,22 @@
         <v>category</v>
       </c>
       <c r="B39" t="str">
-        <v>NeverSummerKey</v>
+        <v>3YearsKey</v>
       </c>
       <c r="C39" t="str">
-        <v>NeverSummerDescription</v>
+        <v>3YearsDescription</v>
       </c>
       <c r="D39" t="str">
-        <v>NeverSummerId</v>
+        <v>3YearsId</v>
       </c>
       <c r="E39" t="str">
-        <v>NeverSummer</v>
+        <v>3Years</v>
       </c>
       <c r="F39" t="str">
-        <v>NeverSummerSlug</v>
+        <v>3YearsSlug</v>
       </c>
       <c r="G39" t="str">
-        <v>brandKey</v>
+        <v>terrainKey</v>
       </c>
       <c r="H39" t="str">
         <v>category</v>
@@ -1421,22 +1421,22 @@
         <v>category</v>
       </c>
       <c r="B40" t="str">
-        <v>child-girlKey</v>
+        <v>YesKey</v>
       </c>
       <c r="C40" t="str">
-        <v>child-girlDescription</v>
+        <v>YesDescription</v>
       </c>
       <c r="D40" t="str">
-        <v>child-girlId</v>
+        <v>YesId</v>
       </c>
       <c r="E40" t="str">
-        <v>Child-girl</v>
+        <v>Yes</v>
       </c>
       <c r="F40" t="str">
-        <v>child-girlSlug</v>
+        <v>YesSlug</v>
       </c>
       <c r="G40" t="str">
-        <v>ageGroupKey</v>
+        <v>brandKey</v>
       </c>
       <c r="H40" t="str">
         <v>category</v>
@@ -1447,19 +1447,19 @@
         <v>category</v>
       </c>
       <c r="B41" t="str">
-        <v>UnitedShapesKey</v>
+        <v>WestonKey</v>
       </c>
       <c r="C41" t="str">
-        <v>UnitedShapesDescription</v>
+        <v>WestonDescription</v>
       </c>
       <c r="D41" t="str">
-        <v>UnitedShapesId</v>
+        <v>WestonId</v>
       </c>
       <c r="E41" t="str">
-        <v>UnitedShapes</v>
+        <v>Weston</v>
       </c>
       <c r="F41" t="str">
-        <v>UnitedShapesSlug</v>
+        <v>WestonSlug</v>
       </c>
       <c r="G41" t="str">
         <v>brandKey</v>
@@ -1473,22 +1473,22 @@
         <v>category</v>
       </c>
       <c r="B42" t="str">
-        <v>3YearsKey</v>
+        <v>CardiffKey</v>
       </c>
       <c r="C42" t="str">
-        <v>3YearsDescription</v>
+        <v>CardiffDescription</v>
       </c>
       <c r="D42" t="str">
-        <v>3YearsId</v>
+        <v>CardiffId</v>
       </c>
       <c r="E42" t="str">
-        <v>3Years</v>
+        <v>Cardiff</v>
       </c>
       <c r="F42" t="str">
-        <v>3YearsSlug</v>
+        <v>CardiffSlug</v>
       </c>
       <c r="G42" t="str">
-        <v>terrainKey</v>
+        <v>brandKey</v>
       </c>
       <c r="H42" t="str">
         <v>category</v>

</xml_diff>